<commit_message>
demux with idemp OM18
</commit_message>
<xml_diff>
--- a/data_raw/map_for_compilation_OM18.xlsx
+++ b/data_raw/map_for_compilation_OM18.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/melo.d/Desktop/Research/Oman_fieldwork/Samail_16S_compilation/data_raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{829C5CEA-A727-6042-9769-78D41A0E7ABA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90123028-1947-814F-86BD-27ED7C1404B9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="16540" xr2:uid="{8FA938D1-D892-E848-A49F-8DF12B7A5192}"/>
   </bookViews>
@@ -428,15 +428,6 @@
     <t>GCTAGTTATGGA</t>
   </si>
   <si>
-    <t>PCR_CNTRL</t>
-  </si>
-  <si>
-    <t>Oman</t>
-  </si>
-  <si>
-    <t>EXT_CNTRL</t>
-  </si>
-  <si>
     <t>NA</t>
   </si>
   <si>
@@ -504,6 +495,15 @@
   </si>
   <si>
     <t>128-131</t>
+  </si>
+  <si>
+    <t>groundwater</t>
+  </si>
+  <si>
+    <t>extraction control</t>
+  </si>
+  <si>
+    <t>PCR control</t>
   </si>
 </sst>
 </file>
@@ -883,10 +883,10 @@
   <dimension ref="A1:V55"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B40" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A2" sqref="A2:XFD2"/>
+      <selection pane="bottomRight" activeCell="E2" sqref="E2:E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -974,61 +974,61 @@
         <v>24</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>131</v>
+        <v>156</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="H2" s="2">
         <v>2018</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="N2" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="O2" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="P2" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="Q2" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="R2" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="S2" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="T2" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="U2" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="V2" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
     </row>
     <row r="3" spans="1:22" ht="17" x14ac:dyDescent="0.25">
@@ -1042,61 +1042,61 @@
         <v>24</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>131</v>
+        <v>156</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="H3" s="2">
         <v>2018</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="L3" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="M3" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="N3" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="O3" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="P3" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="Q3" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="R3" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="S3" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="T3" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="U3" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="V3" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
     </row>
     <row r="4" spans="1:22" ht="17" x14ac:dyDescent="0.25">
@@ -1110,61 +1110,61 @@
         <v>24</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>131</v>
+        <v>156</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="H4" s="2">
         <v>2018</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="L4" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="M4" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="N4" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="O4" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="P4" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="Q4" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="R4" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="S4" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="T4" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="U4" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="V4" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
     </row>
     <row r="5" spans="1:22" ht="17" x14ac:dyDescent="0.25">
@@ -1178,61 +1178,61 @@
         <v>24</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>131</v>
+        <v>156</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="H5" s="2">
         <v>2018</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="L5" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="M5" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="N5" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="O5" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="P5" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="Q5" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="R5" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="S5" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="T5" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="U5" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="V5" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
     </row>
     <row r="6" spans="1:22" ht="17" x14ac:dyDescent="0.25">
@@ -1246,61 +1246,61 @@
         <v>24</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>131</v>
+        <v>156</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="H6" s="2">
         <v>2018</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="L6" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="M6" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="N6" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="O6" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="P6" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="Q6" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="R6" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="S6" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="T6" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="U6" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="V6" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
     </row>
     <row r="7" spans="1:22" ht="17" x14ac:dyDescent="0.25">
@@ -1314,61 +1314,61 @@
         <v>24</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>131</v>
+        <v>156</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="H7" s="2">
         <v>2018</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="L7" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="M7" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="N7" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="O7" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="P7" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="Q7" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="R7" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="S7" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="T7" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="U7" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="V7" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
     </row>
     <row r="8" spans="1:22" ht="17" x14ac:dyDescent="0.25">
@@ -1382,61 +1382,61 @@
         <v>24</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>131</v>
+        <v>156</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="H8" s="2">
         <v>2018</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="J8" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="K8" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="L8" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="M8" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="N8" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="O8" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="P8" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="Q8" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="R8" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="S8" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="T8" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="U8" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="V8" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
     </row>
     <row r="9" spans="1:22" ht="17" x14ac:dyDescent="0.25">
@@ -1450,61 +1450,61 @@
         <v>24</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>131</v>
+        <v>156</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="H9" s="2">
         <v>2018</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="J9" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="K9" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="L9" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="M9" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="N9" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="O9" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="P9" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="Q9" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="R9" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="S9" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="T9" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="U9" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="V9" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
     </row>
     <row r="10" spans="1:22" ht="17" x14ac:dyDescent="0.25">
@@ -1518,61 +1518,61 @@
         <v>24</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>131</v>
+        <v>156</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="H10" s="2">
         <v>2018</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="J10" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="K10" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="L10" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="M10" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="N10" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="O10" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="P10" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="Q10" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="R10" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="S10" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="T10" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="U10" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="V10" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
     </row>
     <row r="11" spans="1:22" ht="17" x14ac:dyDescent="0.25">
@@ -1586,61 +1586,61 @@
         <v>24</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>131</v>
+        <v>156</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="H11" s="2">
         <v>2018</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="J11" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="K11" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="L11" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="M11" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="N11" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="O11" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="P11" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="Q11" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="R11" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="S11" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="T11" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="U11" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="V11" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
     </row>
     <row r="12" spans="1:22" ht="17" x14ac:dyDescent="0.25">
@@ -1654,61 +1654,61 @@
         <v>24</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>131</v>
+        <v>156</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="H12" s="2">
         <v>2018</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="J12" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="K12" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="L12" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="M12" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="N12" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="O12" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="P12" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="Q12" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="R12" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="S12" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="T12" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="U12" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="V12" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
     </row>
     <row r="13" spans="1:22" ht="17" x14ac:dyDescent="0.25">
@@ -1722,61 +1722,61 @@
         <v>24</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>131</v>
+        <v>156</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="H13" s="2">
         <v>2018</v>
       </c>
       <c r="I13" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="J13" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="K13" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="L13" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="M13" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="N13" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="O13" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="P13" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="Q13" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="R13" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="S13" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="T13" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="U13" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="V13" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
     </row>
     <row r="14" spans="1:22" ht="17" x14ac:dyDescent="0.25">
@@ -1790,61 +1790,61 @@
         <v>24</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>131</v>
+        <v>156</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="H14" s="2">
         <v>2018</v>
       </c>
       <c r="I14" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="J14" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="K14" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="L14" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="M14" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="N14" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="O14" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="P14" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="Q14" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="R14" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="S14" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="T14" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="U14" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="V14" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
     </row>
     <row r="15" spans="1:22" ht="17" x14ac:dyDescent="0.25">
@@ -1858,61 +1858,61 @@
         <v>24</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>131</v>
+        <v>156</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="H15" s="2">
         <v>2018</v>
       </c>
       <c r="I15" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="J15" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="K15" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="L15" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="M15" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="N15" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="O15" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="P15" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="Q15" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="R15" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="S15" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="T15" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="U15" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="V15" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
     </row>
     <row r="16" spans="1:22" ht="17" x14ac:dyDescent="0.25">
@@ -1926,61 +1926,61 @@
         <v>24</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>131</v>
+        <v>156</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="H16" s="2">
         <v>2018</v>
       </c>
       <c r="I16" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="J16" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="K16" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="L16" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="M16" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="N16" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="O16" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="P16" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="Q16" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="R16" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="S16" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="T16" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="U16" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="V16" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
     </row>
     <row r="17" spans="1:22" ht="17" x14ac:dyDescent="0.25">
@@ -1994,61 +1994,61 @@
         <v>24</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>131</v>
+        <v>156</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="H17" s="2">
         <v>2018</v>
       </c>
       <c r="I17" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="J17" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="K17" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="L17" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="M17" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="N17" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="O17" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="P17" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="Q17" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="R17" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="S17" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="T17" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="U17" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="V17" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
     </row>
     <row r="18" spans="1:22" ht="17" x14ac:dyDescent="0.25">
@@ -2062,61 +2062,61 @@
         <v>24</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>131</v>
+        <v>156</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="H18" s="2">
         <v>2018</v>
       </c>
       <c r="I18" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="J18" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="K18" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="L18" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="M18" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="N18" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="O18" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="P18" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="Q18" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="R18" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="S18" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="T18" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="U18" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="V18" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
     </row>
     <row r="19" spans="1:22" ht="17" x14ac:dyDescent="0.25">
@@ -2130,61 +2130,61 @@
         <v>24</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>131</v>
+        <v>156</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="H19" s="2">
         <v>2018</v>
       </c>
       <c r="I19" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="J19" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="K19" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="L19" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="M19" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="N19" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="O19" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="P19" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="Q19" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="R19" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="S19" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="T19" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="U19" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="V19" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
     </row>
     <row r="20" spans="1:22" ht="17" x14ac:dyDescent="0.25">
@@ -2198,61 +2198,61 @@
         <v>24</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>131</v>
+        <v>156</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="H20" s="2">
         <v>2018</v>
       </c>
       <c r="I20" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="J20" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="K20" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="L20" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="M20" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="N20" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="O20" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="P20" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="Q20" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="R20" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="S20" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="T20" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="U20" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="V20" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
     </row>
     <row r="21" spans="1:22" ht="17" x14ac:dyDescent="0.25">
@@ -2266,61 +2266,61 @@
         <v>24</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>131</v>
+        <v>156</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="H21" s="2">
         <v>2018</v>
       </c>
       <c r="I21" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="J21" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="K21" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="L21" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="M21" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="N21" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="O21" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="P21" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="Q21" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="R21" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="S21" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="T21" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="U21" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="V21" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
     </row>
     <row r="22" spans="1:22" ht="17" x14ac:dyDescent="0.25">
@@ -2334,16 +2334,16 @@
         <v>24</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>132</v>
+        <v>154</v>
       </c>
       <c r="F22" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="G22" s="3" t="s">
         <v>135</v>
-      </c>
-      <c r="G22" s="3" t="s">
-        <v>138</v>
       </c>
       <c r="H22" s="3">
         <v>2018</v>
@@ -2355,13 +2355,13 @@
         <v>8</v>
       </c>
       <c r="K22" s="5" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="L22" s="5" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="M22" s="5" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="N22" s="5" t="b">
         <v>1</v>
@@ -2373,7 +2373,7 @@
         <v>0</v>
       </c>
       <c r="Q22" s="5" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="R22" s="6">
         <v>400</v>
@@ -2385,7 +2385,7 @@
         <v>1</v>
       </c>
       <c r="U22" s="7" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="V22" s="5">
         <v>13.47</v>
@@ -2402,16 +2402,16 @@
         <v>24</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>132</v>
+        <v>154</v>
       </c>
       <c r="F23" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="G23" s="3" t="s">
         <v>135</v>
-      </c>
-      <c r="G23" s="3" t="s">
-        <v>138</v>
       </c>
       <c r="H23" s="3">
         <v>2018</v>
@@ -2423,13 +2423,13 @@
         <v>8</v>
       </c>
       <c r="K23" s="5" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="L23" s="5" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="M23" s="5" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="N23" s="5" t="b">
         <v>1</v>
@@ -2441,7 +2441,7 @@
         <v>0</v>
       </c>
       <c r="Q23" s="5" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="R23" s="6">
         <v>400</v>
@@ -2453,7 +2453,7 @@
         <v>1</v>
       </c>
       <c r="U23" s="7" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="V23" s="5">
         <v>13.47</v>
@@ -2470,16 +2470,16 @@
         <v>24</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>132</v>
+        <v>154</v>
       </c>
       <c r="F24" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="G24" s="3" t="s">
         <v>135</v>
-      </c>
-      <c r="G24" s="3" t="s">
-        <v>138</v>
       </c>
       <c r="H24" s="3">
         <v>2018</v>
@@ -2491,13 +2491,13 @@
         <v>8</v>
       </c>
       <c r="K24" s="5" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="L24" s="5" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="M24" s="5" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="N24" s="5" t="b">
         <v>1</v>
@@ -2509,7 +2509,7 @@
         <v>0</v>
       </c>
       <c r="Q24" s="5" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="R24" s="6">
         <v>400</v>
@@ -2521,7 +2521,7 @@
         <v>1</v>
       </c>
       <c r="U24" s="7" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="V24" s="5">
         <v>13.47</v>
@@ -2538,16 +2538,16 @@
         <v>24</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>132</v>
+        <v>154</v>
       </c>
       <c r="F25" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="G25" s="3" t="s">
         <v>135</v>
-      </c>
-      <c r="G25" s="3" t="s">
-        <v>138</v>
       </c>
       <c r="H25" s="3">
         <v>2018</v>
@@ -2562,10 +2562,10 @@
         <v>66</v>
       </c>
       <c r="L25" s="5" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="M25" s="5" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="N25" s="5" t="b">
         <v>1</v>
@@ -2589,7 +2589,7 @@
         <v>1</v>
       </c>
       <c r="U25" s="7" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="V25" s="5">
         <v>13.47</v>
@@ -2606,16 +2606,16 @@
         <v>24</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>132</v>
+        <v>154</v>
       </c>
       <c r="F26" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="G26" s="3" t="s">
         <v>135</v>
-      </c>
-      <c r="G26" s="3" t="s">
-        <v>138</v>
       </c>
       <c r="H26" s="3">
         <v>2018</v>
@@ -2630,10 +2630,10 @@
         <v>66</v>
       </c>
       <c r="L26" s="5" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="M26" s="5" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="N26" s="5" t="b">
         <v>1</v>
@@ -2657,7 +2657,7 @@
         <v>1</v>
       </c>
       <c r="U26" s="7" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="V26" s="5">
         <v>13.47</v>
@@ -2674,16 +2674,16 @@
         <v>24</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>132</v>
+        <v>154</v>
       </c>
       <c r="F27" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="G27" s="3" t="s">
         <v>135</v>
-      </c>
-      <c r="G27" s="3" t="s">
-        <v>138</v>
       </c>
       <c r="H27" s="3">
         <v>2018</v>
@@ -2698,10 +2698,10 @@
         <v>66</v>
       </c>
       <c r="L27" s="5" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="M27" s="5" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="N27" s="5" t="b">
         <v>1</v>
@@ -2725,7 +2725,7 @@
         <v>1</v>
       </c>
       <c r="U27" s="7" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="V27" s="5">
         <v>13.47</v>
@@ -2742,16 +2742,16 @@
         <v>24</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>132</v>
+        <v>154</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="G28" s="3" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="H28" s="3">
         <v>2018</v>
@@ -2766,22 +2766,22 @@
         <v>75</v>
       </c>
       <c r="L28" s="5" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="M28" s="5" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="N28" s="5" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="O28" s="5" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="P28" s="5" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="Q28" s="5" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="R28" s="6">
         <v>400</v>
@@ -2793,7 +2793,7 @@
         <v>1</v>
       </c>
       <c r="U28" s="7" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="V28" s="5">
         <v>13.4</v>
@@ -2810,16 +2810,16 @@
         <v>24</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>132</v>
+        <v>154</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="G29" s="3" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="H29" s="3">
         <v>2018</v>
@@ -2834,22 +2834,22 @@
         <v>75</v>
       </c>
       <c r="L29" s="5" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="M29" s="5" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="N29" s="5" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="O29" s="5" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="P29" s="5" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="Q29" s="5" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="R29" s="6">
         <v>400</v>
@@ -2861,7 +2861,7 @@
         <v>1</v>
       </c>
       <c r="U29" s="7" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="V29" s="5">
         <v>13.4</v>
@@ -2878,16 +2878,16 @@
         <v>24</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>132</v>
+        <v>154</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="G30" s="3" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="H30" s="3">
         <v>2018</v>
@@ -2902,22 +2902,22 @@
         <v>75</v>
       </c>
       <c r="L30" s="5" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="M30" s="5" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="N30" s="5" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="O30" s="5" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="P30" s="5" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="Q30" s="5" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="R30" s="6">
         <v>400</v>
@@ -2929,7 +2929,7 @@
         <v>1</v>
       </c>
       <c r="U30" s="7" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="V30" s="5">
         <v>13.4</v>
@@ -2946,16 +2946,16 @@
         <v>24</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>132</v>
+        <v>154</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="G31" s="3" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="H31" s="3">
         <v>2018</v>
@@ -2970,22 +2970,22 @@
         <v>85</v>
       </c>
       <c r="L31" s="5" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="M31" s="5" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="N31" s="5" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="O31" s="5" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="P31" s="5" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="Q31" s="5" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="R31" s="6">
         <v>304</v>
@@ -2997,7 +2997,7 @@
         <v>1</v>
       </c>
       <c r="U31" s="7" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="V31" s="5">
         <v>9.1999999999999993</v>
@@ -3014,16 +3014,16 @@
         <v>24</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>132</v>
+        <v>154</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="G32" s="3" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="H32" s="3">
         <v>2018</v>
@@ -3038,22 +3038,22 @@
         <v>85</v>
       </c>
       <c r="L32" s="5" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="M32" s="5" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="N32" s="5" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="O32" s="5" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="P32" s="5" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="Q32" s="5" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="R32" s="6">
         <v>304</v>
@@ -3065,7 +3065,7 @@
         <v>1</v>
       </c>
       <c r="U32" s="7" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="V32" s="5">
         <v>9.1999999999999993</v>
@@ -3082,16 +3082,16 @@
         <v>24</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>132</v>
+        <v>154</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="G33" s="3" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="H33" s="3">
         <v>2018</v>
@@ -3106,22 +3106,22 @@
         <v>85</v>
       </c>
       <c r="L33" s="5" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="M33" s="5" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="N33" s="5" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="O33" s="5" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="P33" s="5" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="Q33" s="5" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="R33" s="6">
         <v>304</v>
@@ -3133,7 +3133,7 @@
         <v>1</v>
       </c>
       <c r="U33" s="7" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="V33" s="5">
         <v>9.1999999999999993</v>
@@ -3150,16 +3150,16 @@
         <v>24</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>132</v>
+        <v>154</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="G34" s="3" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="H34" s="3">
         <v>2018</v>
@@ -3174,22 +3174,22 @@
         <v>8</v>
       </c>
       <c r="L34" s="5" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="M34" s="5" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="N34" s="5" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="O34" s="5" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="P34" s="5" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="Q34" s="5" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="R34" s="6">
         <v>304</v>
@@ -3201,7 +3201,7 @@
         <v>1</v>
       </c>
       <c r="U34" s="7" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="V34" s="5">
         <v>4.7</v>
@@ -3218,61 +3218,61 @@
         <v>24</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>133</v>
+        <v>155</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="G35" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="H35" s="2">
         <v>2018</v>
       </c>
       <c r="I35" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="J35" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="K35" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="L35" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="M35" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="N35" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="O35" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="P35" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="Q35" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="R35" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="S35" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="T35" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="U35" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="V35" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
     </row>
     <row r="36" spans="1:22" ht="17" x14ac:dyDescent="0.25">
@@ -3286,61 +3286,61 @@
         <v>24</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>133</v>
+        <v>155</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="G36" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="H36" s="2">
         <v>2018</v>
       </c>
       <c r="I36" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="J36" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="K36" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="L36" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="M36" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="N36" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="O36" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="P36" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="Q36" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="R36" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="S36" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="T36" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="U36" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="V36" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
     </row>
     <row r="37" spans="1:22" ht="17" x14ac:dyDescent="0.25">
@@ -3354,61 +3354,61 @@
         <v>24</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>133</v>
+        <v>155</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="G37" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="H37" s="2">
         <v>2018</v>
       </c>
       <c r="I37" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="J37" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="K37" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="L37" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="M37" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="N37" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="O37" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="P37" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="Q37" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="R37" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="S37" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="T37" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="U37" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="V37" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
     </row>
     <row r="38" spans="1:22" ht="17" x14ac:dyDescent="0.25">
@@ -3422,16 +3422,16 @@
         <v>24</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>132</v>
+        <v>154</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="G38" s="3" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="H38" s="3">
         <v>2018</v>
@@ -3446,22 +3446,22 @@
         <v>70</v>
       </c>
       <c r="L38" s="5" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="M38" s="5" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="N38" s="5" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="O38" s="5" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="P38" s="5" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="Q38" s="5" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="R38" s="6">
         <v>101</v>
@@ -3473,7 +3473,7 @@
         <v>1</v>
       </c>
       <c r="U38" s="7" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="V38" s="5">
         <v>15</v>
@@ -3490,16 +3490,16 @@
         <v>24</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>132</v>
+        <v>154</v>
       </c>
       <c r="F39" s="2" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="G39" s="3" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="H39" s="3">
         <v>2018</v>
@@ -3514,22 +3514,22 @@
         <v>70</v>
       </c>
       <c r="L39" s="5" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="M39" s="5" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="N39" s="5" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="O39" s="5" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="P39" s="5" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="Q39" s="5" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="R39" s="6">
         <v>101</v>
@@ -3541,7 +3541,7 @@
         <v>1</v>
       </c>
       <c r="U39" s="7" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="V39" s="5">
         <v>15</v>
@@ -3558,16 +3558,16 @@
         <v>24</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>132</v>
+        <v>154</v>
       </c>
       <c r="F40" s="2" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="G40" s="3" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="H40" s="3">
         <v>2018</v>
@@ -3582,22 +3582,22 @@
         <v>70</v>
       </c>
       <c r="L40" s="5" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="M40" s="5" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="N40" s="5" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="O40" s="5" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="P40" s="5" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="Q40" s="5" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="R40" s="6">
         <v>101</v>
@@ -3609,7 +3609,7 @@
         <v>1</v>
       </c>
       <c r="U40" s="7" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="V40" s="5">
         <v>15</v>
@@ -3626,16 +3626,16 @@
         <v>24</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>132</v>
+        <v>154</v>
       </c>
       <c r="F41" s="2" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="G41" s="3" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="H41" s="3">
         <v>2018</v>
@@ -3650,22 +3650,22 @@
         <v>85</v>
       </c>
       <c r="L41" s="5" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="M41" s="5" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="N41" s="5" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="O41" s="5" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="P41" s="5" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="Q41" s="5" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="R41" s="6">
         <v>120.4</v>
@@ -3677,7 +3677,7 @@
         <v>1</v>
       </c>
       <c r="U41" s="7" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="V41" s="5">
         <v>40</v>
@@ -3694,16 +3694,16 @@
         <v>24</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>132</v>
+        <v>154</v>
       </c>
       <c r="F42" s="2" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="G42" s="3" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="H42" s="3">
         <v>2018</v>
@@ -3718,22 +3718,22 @@
         <v>85</v>
       </c>
       <c r="L42" s="5" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="M42" s="5" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="N42" s="5" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="O42" s="5" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="P42" s="5" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="Q42" s="5" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="R42" s="6">
         <v>120.4</v>
@@ -3745,7 +3745,7 @@
         <v>1</v>
       </c>
       <c r="U42" s="7" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="V42" s="5">
         <v>40</v>
@@ -3762,16 +3762,16 @@
         <v>24</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>132</v>
+        <v>154</v>
       </c>
       <c r="F43" s="2" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="G43" s="3" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="H43" s="3">
         <v>2018</v>
@@ -3786,22 +3786,22 @@
         <v>85</v>
       </c>
       <c r="L43" s="5" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="M43" s="5" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="N43" s="5" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="O43" s="5" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="P43" s="5" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="Q43" s="5" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="R43" s="6">
         <v>120.4</v>
@@ -3813,7 +3813,7 @@
         <v>1</v>
       </c>
       <c r="U43" s="7" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="V43" s="5">
         <v>40</v>
@@ -3830,16 +3830,16 @@
         <v>24</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>132</v>
+        <v>154</v>
       </c>
       <c r="F44" s="2" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="G44" s="3" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="H44" s="3">
         <v>2018</v>
@@ -3854,22 +3854,22 @@
         <v>60</v>
       </c>
       <c r="L44" s="5" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="M44" s="5" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="N44" s="5" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="O44" s="5" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="P44" s="5" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="Q44" s="5" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="R44" s="6">
         <v>120.5</v>
@@ -3881,7 +3881,7 @@
         <v>1</v>
       </c>
       <c r="U44" s="7" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="V44" s="5">
         <v>16.5</v>
@@ -3898,16 +3898,16 @@
         <v>24</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>132</v>
+        <v>154</v>
       </c>
       <c r="F45" s="2" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="G45" s="3" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="H45" s="3">
         <v>2018</v>
@@ -3922,22 +3922,22 @@
         <v>60</v>
       </c>
       <c r="L45" s="5" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="M45" s="5" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="N45" s="5" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="O45" s="5" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="P45" s="5" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="Q45" s="5" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="R45" s="6">
         <v>120.5</v>
@@ -3949,7 +3949,7 @@
         <v>1</v>
       </c>
       <c r="U45" s="7" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="V45" s="5">
         <v>16.5</v>
@@ -3966,16 +3966,16 @@
         <v>24</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>132</v>
+        <v>154</v>
       </c>
       <c r="F46" s="2" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="G46" s="3" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="H46" s="3">
         <v>2018</v>
@@ -3990,22 +3990,22 @@
         <v>60</v>
       </c>
       <c r="L46" s="5" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="M46" s="5" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="N46" s="5" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="O46" s="5" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="P46" s="5" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="Q46" s="5" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="R46" s="6">
         <v>120.5</v>
@@ -4017,7 +4017,7 @@
         <v>1</v>
       </c>
       <c r="U46" s="7" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="V46" s="5">
         <v>16.5</v>
@@ -4034,16 +4034,16 @@
         <v>24</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="E47" s="2" t="s">
-        <v>132</v>
+        <v>154</v>
       </c>
       <c r="F47" s="2" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="G47" s="3" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="H47" s="3">
         <v>2018</v>
@@ -4058,22 +4058,22 @@
         <v>50</v>
       </c>
       <c r="L47" s="5" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="M47" s="5" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="N47" s="5" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="O47" s="5" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="P47" s="5" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="Q47" s="5" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="R47" s="6">
         <v>78</v>
@@ -4085,7 +4085,7 @@
         <v>1</v>
       </c>
       <c r="U47" s="7" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="V47" s="5">
         <v>9.5</v>
@@ -4102,16 +4102,16 @@
         <v>24</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="E48" s="2" t="s">
-        <v>132</v>
+        <v>154</v>
       </c>
       <c r="F48" s="2" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="G48" s="3" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="H48" s="3">
         <v>2018</v>
@@ -4126,22 +4126,22 @@
         <v>50</v>
       </c>
       <c r="L48" s="5" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="M48" s="5" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="N48" s="5" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="O48" s="5" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="P48" s="5" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="Q48" s="5" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="R48" s="6">
         <v>78</v>
@@ -4153,7 +4153,7 @@
         <v>1</v>
       </c>
       <c r="U48" s="7" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="V48" s="5">
         <v>9.5</v>
@@ -4170,16 +4170,16 @@
         <v>24</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="E49" s="2" t="s">
-        <v>132</v>
+        <v>154</v>
       </c>
       <c r="F49" s="2" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="G49" s="3" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="H49" s="3">
         <v>2018</v>
@@ -4194,22 +4194,22 @@
         <v>50</v>
       </c>
       <c r="L49" s="5" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="M49" s="5" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="N49" s="5" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="O49" s="5" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="P49" s="5" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="Q49" s="5" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="R49" s="6">
         <v>78</v>
@@ -4221,7 +4221,7 @@
         <v>1</v>
       </c>
       <c r="U49" s="7" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="V49" s="5">
         <v>9.5</v>
@@ -4238,16 +4238,16 @@
         <v>24</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="E50" s="2" t="s">
-        <v>132</v>
+        <v>154</v>
       </c>
       <c r="F50" s="2" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="G50" s="3" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="H50" s="3">
         <v>2018</v>
@@ -4262,22 +4262,22 @@
         <v>50</v>
       </c>
       <c r="L50" s="5" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="M50" s="5" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="N50" s="5" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="O50" s="5" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="P50" s="5" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="Q50" s="5" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="R50" s="6">
         <v>102</v>
@@ -4289,7 +4289,7 @@
         <v>1</v>
       </c>
       <c r="U50" s="7" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="V50" s="5">
         <v>7.5</v>
@@ -4306,16 +4306,16 @@
         <v>24</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="E51" s="2" t="s">
-        <v>132</v>
+        <v>154</v>
       </c>
       <c r="F51" s="2" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="G51" s="3" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="H51" s="3">
         <v>2018</v>
@@ -4330,22 +4330,22 @@
         <v>50</v>
       </c>
       <c r="L51" s="5" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="M51" s="5" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="N51" s="5" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="O51" s="5" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="P51" s="5" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="Q51" s="5" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="R51" s="6">
         <v>102</v>
@@ -4357,7 +4357,7 @@
         <v>1</v>
       </c>
       <c r="U51" s="7" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="V51" s="5">
         <v>7.5</v>
@@ -4374,16 +4374,16 @@
         <v>24</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="E52" s="2" t="s">
-        <v>132</v>
+        <v>154</v>
       </c>
       <c r="F52" s="2" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="G52" s="3" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="H52" s="3">
         <v>2018</v>
@@ -4398,22 +4398,22 @@
         <v>50</v>
       </c>
       <c r="L52" s="5" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="M52" s="5" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="N52" s="5" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="O52" s="5" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="P52" s="5" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="Q52" s="5" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="R52" s="6">
         <v>102</v>
@@ -4425,7 +4425,7 @@
         <v>1</v>
       </c>
       <c r="U52" s="7" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="V52" s="5">
         <v>7.5</v>
@@ -4442,16 +4442,16 @@
         <v>24</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="E53" s="2" t="s">
-        <v>132</v>
+        <v>154</v>
       </c>
       <c r="F53" s="2" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="G53" s="3" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="H53" s="3">
         <v>2018</v>
@@ -4466,22 +4466,22 @@
         <v>70</v>
       </c>
       <c r="L53" s="5" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="M53" s="5" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="N53" s="5" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="O53" s="5" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="P53" s="5" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="Q53" s="5" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="R53" s="6">
         <v>136.5</v>
@@ -4493,7 +4493,7 @@
         <v>1</v>
       </c>
       <c r="U53" s="7" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="V53" s="5">
         <v>8.3000000000000007</v>
@@ -4510,16 +4510,16 @@
         <v>24</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="E54" s="2" t="s">
-        <v>132</v>
+        <v>154</v>
       </c>
       <c r="F54" s="2" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="G54" s="3" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="H54" s="3">
         <v>2018</v>
@@ -4534,22 +4534,22 @@
         <v>70</v>
       </c>
       <c r="L54" s="5" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="M54" s="5" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="N54" s="5" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="O54" s="5" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="P54" s="5" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="Q54" s="5" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="R54" s="6">
         <v>136.5</v>
@@ -4561,7 +4561,7 @@
         <v>1</v>
       </c>
       <c r="U54" s="7" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="V54" s="5">
         <v>8.3000000000000007</v>
@@ -4578,16 +4578,16 @@
         <v>24</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="E55" s="2" t="s">
-        <v>132</v>
+        <v>154</v>
       </c>
       <c r="F55" s="2" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="G55" s="3" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="H55" s="3">
         <v>2018</v>
@@ -4602,22 +4602,22 @@
         <v>70</v>
       </c>
       <c r="L55" s="5" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="M55" s="5" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="N55" s="5" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="O55" s="5" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="P55" s="5" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="Q55" s="5" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="R55" s="6">
         <v>136.5</v>
@@ -4629,7 +4629,7 @@
         <v>1</v>
       </c>
       <c r="U55" s="7" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="V55" s="5">
         <v>8.3000000000000007</v>

</xml_diff>